<commit_message>
updated spreadsheet for ExC
</commit_message>
<xml_diff>
--- a/IEP_Exercise C plots_V2.xlsx
+++ b/IEP_Exercise C plots_V2.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joebrakoniecki/Documents/Cambridge/Coursework/IEP/Ex C/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E5F4EB-FBF9-9449-9571-F644D8233997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AA1D38-C087-8247-9C63-5F574FF904B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{0B9BCFD2-083C-DD4F-BFCB-A2665170C659}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" activeTab="4" xr2:uid="{0B9BCFD2-083C-DD4F-BFCB-A2665170C659}"/>
   </bookViews>
   <sheets>
     <sheet name="Data (frequency response)" sheetId="2" r:id="rId1"/>
-    <sheet name="Graph (gain vs freq) (2)" sheetId="12" r:id="rId2"/>
+    <sheet name="Attenuation vs Frequncy" sheetId="12" state="hidden" r:id="rId2"/>
     <sheet name="Graph (gain vs freq)" sheetId="7" r:id="rId3"/>
     <sheet name="Graph (phase vs freq)" sheetId="8" r:id="rId4"/>
+    <sheet name="Graph (gain vs freq) Tol" sheetId="13" r:id="rId5"/>
+    <sheet name="Graph (phase vs freq) tol" sheetId="14" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Data (frequency response)'!$B$15</definedName>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>RMS A (mV)</t>
   </si>
@@ -147,7 +149,10 @@
     <t>Gain and phase (from experiment and theory)</t>
   </si>
   <si>
-    <t>Attenuation</t>
+    <t>RC time constant (s) Max</t>
+  </si>
+  <si>
+    <t>RC time constant (s) Min</t>
   </si>
 </sst>
 </file>
@@ -314,7 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -350,6 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,9 +410,6 @@
               <c:f>'Data (frequency response)'!$L$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Attenuation</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -482,36 +484,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.99433656957928807</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.99183673469387756</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.95198675496688745</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.94572368421052633</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62446290461185905</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.30675984027381631</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.16065059209587673</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.1417569880205362E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.3504419731964642E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.7078042516764161E-2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1683,7 +1655,7 @@
                   <c:v>-51.488112746033423</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-72.343212848587157</c:v>
+                  <c:v>-72.343212848587129</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-80.956938920962315</c:v>
@@ -2070,6 +2042,1706 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12611647093601358"/>
+          <c:y val="7.6235643319454191E-2"/>
+          <c:w val="0.83395178844965201"/>
+          <c:h val="0.80863338417776309"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured gain (dB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$H$4:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-4.93317573268586E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.1196215324405482E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.42738187863002647</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.48471469166208891</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.0898671041914803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10.264029940685894</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15.882353389364338</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-21.785637288301487</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-29.497957985474947</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-35.35123819154267</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D4F-BC45-ADE4-787B76B4AF57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical gain with RC=0.1 s (dB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$I$4:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1.7111504344581821E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.8045175474464911E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.40877560788352169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.445070116205287</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.1147436202747096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10.362137382398966</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-16.072235265805517</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-22.011612586390065</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-29.947395549253176</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-35.964697308632864</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D4F-BC45-ADE4-787B76B4AF57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical gain with RC=0.115 s (dB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-2.2615617856389846E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.9764325772805298E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.53280369680303707</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.8244377738529742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.8973470970916679</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-11.47755195480004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-17.259949507336007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-23.218899935782538</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-31.160280263478981</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-37.178385913694818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2D4F-BC45-ADE4-787B76B4AF57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical gain with RC=0.085 s (dB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$P$4:$P$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1.2369816633159818E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.9269266701835179E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.299143041578879</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.0898138392640417</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.3060171090981427</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.101327005501691</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-14.701627919183222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-20.61047502523142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-28.537462114242025</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-34.55349821775129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-2D4F-BC45-ADE4-787B76B4AF57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="298120623"/>
+        <c:axId val="896715823"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="298120623"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" cap="none" baseline="0"/>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896715823"/>
+        <c:crossesAt val="-60"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="896715823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" cap="none" baseline="0"/>
+                  <a:t>Gain (dB)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="298120623"/>
+        <c:crossesAt val="0.1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15290102389078497"/>
+          <c:y val="0.4119419548996166"/>
+          <c:w val="0.32616912723282621"/>
+          <c:h val="0.41427060788441206"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13157722178925588"/>
+          <c:y val="7.6235643319454191E-2"/>
+          <c:w val="0.83395178844965201"/>
+          <c:h val="0.80863338417776309"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Measured phase (degrees)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$J$4:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-4.4280000000000008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.3231999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-17.985600000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-32.817599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-48.362400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-68.706000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-77.867999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-84.024000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-86.076000000000022</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-101.73599999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4223-C549-9BAC-F4FE180E89A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical phase with RC=0.1 s (degrees)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$K$4:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-3.5952737798681755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.1624558067258226</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-17.44059449051187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-32.141907635342058</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-51.488112746033423</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-72.343212848587129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-80.956938920962315</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-85.450134690878912</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-88.176834279185869</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-89.088186330386165</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4223-C549-9BAC-F4FE180E89A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical phase with RC=0.115 s (degrees)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$M$4:$M$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-4.132817478062857</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.2230715851746758</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-19.863934154775816</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-35.850607418335656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-55.317617543297104</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-74.528379606257459</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-82.120567493147149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-86.04156808434314</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-88.41450802948313</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-89.207102225835101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4223-C549-9BAC-F4FE180E89A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data (frequency response)'!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Theoretical phase with RC=0.085 s (degrees)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+                <a:noFill/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$A$4:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data (frequency response)'!$N$4:$N$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-3.0570956069442095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.0968831467209785</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.95113830986352</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-28.105371183101663</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-46.887109086835764</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-69.469968336749645</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-79.394674953870918</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-84.651527093870286</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-87.855377077800327</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-88.927312814232252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4223-C549-9BAC-F4FE180E89A8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="298120623"/>
+        <c:axId val="896715823"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="298120623"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" cap="none" baseline="0"/>
+                  <a:t>Frequency (Hz)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="896715823"/>
+        <c:crossesAt val="-90"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="896715823"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" cap="none" baseline="0"/>
+                  <a:t>Phase (degrees)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.3767058127972907E-2"/>
+              <c:y val="0.35952096302098357"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="298120623"/>
+        <c:crossesAt val="0.1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.65801426807329411"/>
+          <c:y val="7.4824499853406723E-2"/>
+          <c:w val="0.30694104530491645"/>
+          <c:h val="0.41427060788441206"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2190,6 +3862,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
   <cs:axisTitle>
@@ -3738,11 +5490,1043 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="70000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="2000" kern="1200" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="38100" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1471938A-2842-BA42-93C9-1DEFD9549165}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3753,7 +6537,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{90A2F41D-51E9-3541-A87E-54C1ED69F698}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3764,7 +6548,29 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C551B57A-0C4F-4746-9CB0-EA6D01C74747}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="124" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{727D9578-6F1B-A54A-8ECB-A3432E08CDDF}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E04DD220-D072-1446-B851-FDAA46DCC254}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3775,7 +6581,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309919" cy="6073468"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3808,7 +6614,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309919" cy="6073468"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -3841,13 +6647,79 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9309919" cy="6073468"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{273EB7CB-EBF9-4844-8ADC-57E63688E870}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290A2C3C-9242-9A57-F732-F561285F6AFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9303008" cy="6071220"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03E18279-E4E0-19A7-7053-C01836BDFB58}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4167,15 +7039,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DA2538-D0A7-5C42-9EEB-DECA1BBAFEB3}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
@@ -4187,7 +7059,7 @@
     <col min="12" max="12" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.83203125" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" customWidth="1"/>
     <col min="16" max="16" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="20.83203125" customWidth="1"/>
@@ -4197,569 +7069,716 @@
     <col min="24" max="24" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
     </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:16" s="4" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="16" t="str">
+      <c r="I3" s="15" t="str">
         <f>_xlfn.CONCAT("Theoretical gain with RC=",B15," s (dB)")</f>
         <v>Theoretical gain with RC=0.1 s (dB)</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="16" t="str">
+      <c r="K3" s="15" t="str">
         <f>_xlfn.CONCAT("Theoretical phase with RC=",B15," s (degrees)")</f>
         <v>Theoretical phase with RC=0.1 s (degrees)</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>27</v>
+      <c r="M3" s="15" t="str">
+        <f>_xlfn.CONCAT("Theoretical phase with RC=",B16," s (degrees)")</f>
+        <v>Theoretical phase with RC=0.115 s (degrees)</v>
+      </c>
+      <c r="N3" s="15" t="str">
+        <f>_xlfn.CONCAT("Theoretical phase with RC=",B17," s (degrees)")</f>
+        <v>Theoretical phase with RC=0.085 s (degrees)</v>
+      </c>
+      <c r="O3" s="15" t="str">
+        <f>_xlfn.CONCAT("Theoretical gain with RC=",B16," s (dB)")</f>
+        <v>Theoretical gain with RC=0.115 s (dB)</v>
+      </c>
+      <c r="P3" s="15" t="str">
+        <f>_xlfn.CONCAT("Theoretical gain with RC=",B17," s (dB)")</f>
+        <v>Theoretical gain with RC=0.085 s (dB)</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
         <v>0.1</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>1236</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>1229</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>123</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <f>IF(ISBLANK(B4),NA(),20*LOG10($C4/$B4))</f>
         <v>-4.93317573268586E-2</v>
       </c>
-      <c r="I4" s="15">
-        <f t="shared" ref="I4:I13" si="0">-10*LOG10((1+(2*PI()*$A4*$B$15)^2))</f>
+      <c r="I4" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A4*$B$15)^2))</f>
         <v>-1.7111504344581821E-2</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="14">
         <f>IF(ISBLANK(D4),NA(),-2*PI()*$D4*$A4/1000*180/PI())</f>
         <v>-4.4280000000000008</v>
       </c>
-      <c r="K4" s="15">
-        <f t="shared" ref="K4:K13" si="1">-ATAN($A4*2*PI()*$B$15)*180/PI()</f>
+      <c r="K4" s="14">
+        <f>-ATAN($A4*2*PI()*$B$15)*180/PI()</f>
         <v>-3.5952737798681755</v>
       </c>
-      <c r="L4">
-        <f>C4/B4</f>
-        <v>0.99433656957928807</v>
+      <c r="M4" s="14">
+        <f>-ATAN($A4*2*PI()*$B$16)*180/PI()</f>
+        <v>-4.132817478062857</v>
+      </c>
+      <c r="N4" s="14">
+        <f>-ATAN($A4*2*PI()*$B$17)*180/PI()</f>
+        <v>-3.0570956069442095</v>
+      </c>
+      <c r="O4" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A4*$B$16)^2))</f>
+        <v>-2.2615617856389846E-2</v>
+      </c>
+      <c r="P4" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A4*$B$17)^2))</f>
+        <v>-1.2369816633159818E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>0.2</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>1225</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>1215</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>115.6</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <f>IF(ISBLANK(B5),NA(),20*LOG10($C5/$B5))</f>
         <v>-7.1196215324405482E-2</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A5*$B$15)^2))</f>
+        <v>-6.8045175474464911E-2</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" ref="J5:J13" si="0">IF(ISBLANK(D5),NA(),-2*PI()*$D5*$A5/1000*180/PI())</f>
+        <v>-8.3231999999999999</v>
+      </c>
+      <c r="K5" s="7">
+        <f>-ATAN($A5*2*PI()*$B$15)*180/PI()</f>
+        <v>-7.1624558067258226</v>
+      </c>
+      <c r="M5" s="14">
+        <f>-ATAN($A5*2*PI()*$B$16)*180/PI()</f>
+        <v>-8.2230715851746758</v>
+      </c>
+      <c r="N5" s="14">
+        <f t="shared" ref="N5:N13" si="1">-ATAN($A5*2*PI()*$B$17)*180/PI()</f>
+        <v>-6.0968831467209785</v>
+      </c>
+      <c r="O5" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A5*$B$16)^2))</f>
+        <v>-8.9764325772805298E-2</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" ref="P5:P13" si="2">-10*LOG10((1+(2*PI()*$A5*$B$17)^2))</f>
+        <v>-4.9269266701835179E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1208</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1150</v>
+      </c>
+      <c r="D6" s="6">
+        <v>99.92</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" ref="H6:H13" si="3">IF(ISBLANK(B6),NA(),20*LOG10($C6/$B6))</f>
+        <v>-0.42738187863002647</v>
+      </c>
+      <c r="I6" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A6*$B$15)^2))</f>
+        <v>-0.40877560788352169</v>
+      </c>
+      <c r="J6" s="7">
+        <f>IF(ISBLANK(D6),NA(),-2*PI()*$D6*$A6/1000*180/PI())</f>
+        <v>-17.985600000000002</v>
+      </c>
+      <c r="K6" s="7">
+        <f>-ATAN($A6*2*PI()*$B$15)*180/PI()</f>
+        <v>-17.44059449051187</v>
+      </c>
+      <c r="M6" s="14">
+        <f>-ATAN($A6*2*PI()*$B$16)*180/PI()</f>
+        <v>-19.863934154775816</v>
+      </c>
+      <c r="N6" s="14">
+        <f t="shared" si="1"/>
+        <v>-14.95113830986352</v>
+      </c>
+      <c r="O6" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A6*$B$16)^2))</f>
+        <v>-0.53280369680303707</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" si="2"/>
+        <v>-0.299143041578879</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1216</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1150</v>
+      </c>
+      <c r="D7" s="6">
+        <v>91.16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="3"/>
+        <v>-0.48471469166208891</v>
+      </c>
+      <c r="I7" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A7*$B$15)^2))</f>
+        <v>-1.445070116205287</v>
+      </c>
+      <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>-6.8045175474464911E-2</v>
-      </c>
-      <c r="J5" s="8">
-        <f t="shared" ref="J5:J13" si="2">IF(ISBLANK(D5),NA(),-2*PI()*$D5*$A5/1000*180/PI())</f>
-        <v>-8.3231999999999999</v>
-      </c>
-      <c r="K5" s="8">
+        <v>-32.817599999999999</v>
+      </c>
+      <c r="K7" s="7">
+        <f>-ATAN($A7*2*PI()*$B$15)*180/PI()</f>
+        <v>-32.141907635342058</v>
+      </c>
+      <c r="M7" s="14">
+        <f>-ATAN($A7*2*PI()*$B$16)*180/PI()</f>
+        <v>-35.850607418335656</v>
+      </c>
+      <c r="N7" s="14">
         <f t="shared" si="1"/>
-        <v>-7.1624558067258226</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L13" si="3">C5/B5</f>
-        <v>0.99183673469387756</v>
+        <v>-28.105371183101663</v>
+      </c>
+      <c r="O7" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A7*$B$16)^2))</f>
+        <v>-1.8244377738529742</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="2"/>
+        <v>-1.0898138392640417</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1208</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1150</v>
-      </c>
-      <c r="D6" s="7">
-        <v>99.92</v>
-      </c>
-      <c r="E6" s="6" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>698.2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>436</v>
+      </c>
+      <c r="D8" s="6">
+        <v>67.17</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="3"/>
+        <v>-4.0898671041914803</v>
+      </c>
+      <c r="I8" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A8*$B$15)^2))</f>
+        <v>-4.1147436202747096</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="0"/>
+        <v>-48.362400000000001</v>
+      </c>
+      <c r="K8" s="7">
+        <f>-ATAN($A8*2*PI()*$B$15)*180/PI()</f>
+        <v>-51.488112746033423</v>
+      </c>
+      <c r="M8" s="14">
+        <f>-ATAN($A8*2*PI()*$B$16)*180/PI()</f>
+        <v>-55.317617543297104</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="1"/>
+        <v>-46.887109086835764</v>
+      </c>
+      <c r="O8" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A8*$B$16)^2))</f>
+        <v>-4.8973470970916679</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="2"/>
+        <v>-3.3060171090981427</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7">
+        <v>701.2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>215.1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>38.17</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="3"/>
+        <v>-10.264029940685894</v>
+      </c>
+      <c r="I9" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A9*$B$15)^2))</f>
+        <v>-10.362137382398966</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="0"/>
+        <v>-68.706000000000003</v>
+      </c>
+      <c r="K9" s="7">
+        <f>-ATAN($A9*2*PI()*$B$15)*180/PI()</f>
+        <v>-72.343212848587129</v>
+      </c>
+      <c r="M9" s="14">
+        <f>-ATAN($A9*2*PI()*$B$16)*180/PI()</f>
+        <v>-74.528379606257459</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="1"/>
+        <v>-69.469968336749645</v>
+      </c>
+      <c r="O9" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A9*$B$16)^2))</f>
+        <v>-11.47755195480004</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="2"/>
+        <v>-9.101327005501691</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7">
+        <v>700.9</v>
+      </c>
+      <c r="C10" s="7">
+        <v>112.6</v>
+      </c>
+      <c r="D10" s="6">
+        <v>21.63</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="3"/>
+        <v>-15.882353389364338</v>
+      </c>
+      <c r="I10" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A10*$B$15)^2))</f>
+        <v>-16.072235265805517</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="0"/>
+        <v>-77.867999999999995</v>
+      </c>
+      <c r="K10" s="7">
+        <f>-ATAN($A10*2*PI()*$B$15)*180/PI()</f>
+        <v>-80.956938920962315</v>
+      </c>
+      <c r="M10" s="14">
+        <f>-ATAN($A10*2*PI()*$B$16)*180/PI()</f>
+        <v>-82.120567493147149</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="1"/>
+        <v>-79.394674953870918</v>
+      </c>
+      <c r="O10" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A10*$B$16)^2))</f>
+        <v>-17.259949507336007</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="2"/>
+        <v>-14.701627919183222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>20</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="10">
-        <f t="shared" ref="H5:H13" si="4">IF(ISBLANK(B6),NA(),20*LOG10($C6/$B6))</f>
-        <v>-0.42738187863002647</v>
-      </c>
-      <c r="I6" s="8">
+      <c r="B11" s="7">
+        <v>701.2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>57.09</v>
+      </c>
+      <c r="D11" s="6">
+        <v>11.67</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="3"/>
+        <v>-21.785637288301487</v>
+      </c>
+      <c r="I11" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A11*$B$15)^2))</f>
+        <v>-22.011612586390065</v>
+      </c>
+      <c r="J11" s="7">
         <f t="shared" si="0"/>
-        <v>-0.40877560788352169</v>
-      </c>
-      <c r="J6" s="8">
+        <v>-84.024000000000001</v>
+      </c>
+      <c r="K11" s="7">
+        <f>-ATAN($A11*2*PI()*$B$15)*180/PI()</f>
+        <v>-85.450134690878912</v>
+      </c>
+      <c r="M11" s="14">
+        <f>-ATAN($A11*2*PI()*$B$16)*180/PI()</f>
+        <v>-86.04156808434314</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="1"/>
+        <v>-84.651527093870286</v>
+      </c>
+      <c r="O11" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A11*$B$16)^2))</f>
+        <v>-23.218899935782538</v>
+      </c>
+      <c r="P11" s="14">
         <f t="shared" si="2"/>
-        <v>-17.985600000000002</v>
-      </c>
-      <c r="K6" s="8">
+        <v>-20.61047502523142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>50</v>
+      </c>
+      <c r="B12" s="7">
+        <v>701.4</v>
+      </c>
+      <c r="C12" s="7">
+        <v>23.5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>4.782</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="3"/>
+        <v>-29.497957985474947</v>
+      </c>
+      <c r="I12" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A12*$B$15)^2))</f>
+        <v>-29.947395549253176</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="0"/>
+        <v>-86.076000000000022</v>
+      </c>
+      <c r="K12" s="7">
+        <f>-ATAN($A12*2*PI()*$B$15)*180/PI()</f>
+        <v>-88.176834279185869</v>
+      </c>
+      <c r="M12" s="14">
+        <f>-ATAN($A12*2*PI()*$B$16)*180/PI()</f>
+        <v>-88.41450802948313</v>
+      </c>
+      <c r="N12" s="14">
         <f t="shared" si="1"/>
-        <v>-17.44059449051187</v>
-      </c>
-      <c r="L6">
+        <v>-87.855377077800327</v>
+      </c>
+      <c r="O12" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A12*$B$16)^2))</f>
+        <v>-31.160280263478981</v>
+      </c>
+      <c r="P12" s="14">
+        <f t="shared" si="2"/>
+        <v>-28.537462114242025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>100</v>
+      </c>
+      <c r="B13" s="7">
+        <v>700.9</v>
+      </c>
+      <c r="C13" s="7">
+        <v>11.97</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.8260000000000001</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="9">
         <f t="shared" si="3"/>
-        <v>0.95198675496688745</v>
+        <v>-35.35123819154267</v>
+      </c>
+      <c r="I13" s="7">
+        <f>-10*LOG10((1+(2*PI()*$A13*$B$15)^2))</f>
+        <v>-35.964697308632864</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="0"/>
+        <v>-101.73599999999999</v>
+      </c>
+      <c r="K13" s="7">
+        <f>-ATAN($A13*2*PI()*$B$15)*180/PI()</f>
+        <v>-89.088186330386165</v>
+      </c>
+      <c r="M13" s="14">
+        <f>-ATAN($A13*2*PI()*$B$16)*180/PI()</f>
+        <v>-89.207102225835101</v>
+      </c>
+      <c r="N13" s="14">
+        <f t="shared" si="1"/>
+        <v>-88.927312814232252</v>
+      </c>
+      <c r="O13" s="14">
+        <f>-10*LOG10((1+(2*PI()*$A13*$B$16)^2))</f>
+        <v>-37.178385913694818</v>
+      </c>
+      <c r="P13" s="14">
+        <f t="shared" si="2"/>
+        <v>-34.55349821775129</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>1</v>
-      </c>
-      <c r="B7" s="8">
-        <v>1216</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1150</v>
-      </c>
-      <c r="D7" s="7">
-        <v>91.16</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="10">
-        <f t="shared" si="4"/>
-        <v>-0.48471469166208891</v>
-      </c>
-      <c r="I7" s="8">
-        <f t="shared" si="0"/>
-        <v>-1.445070116205287</v>
-      </c>
-      <c r="J7" s="8">
-        <f t="shared" si="2"/>
-        <v>-32.817599999999999</v>
-      </c>
-      <c r="K7" s="8">
-        <f t="shared" si="1"/>
-        <v>-32.141907635342058</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="3"/>
-        <v>0.94572368421052633</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>2</v>
-      </c>
-      <c r="B8" s="8">
-        <v>698.2</v>
-      </c>
-      <c r="C8" s="8">
-        <v>436</v>
-      </c>
-      <c r="D8" s="7">
-        <v>67.17</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="10">
-        <f t="shared" si="4"/>
-        <v>-4.0898671041914803</v>
-      </c>
-      <c r="I8" s="8">
-        <f t="shared" si="0"/>
-        <v>-4.1147436202747096</v>
-      </c>
-      <c r="J8" s="8">
-        <f t="shared" si="2"/>
-        <v>-48.362400000000001</v>
-      </c>
-      <c r="K8" s="8">
-        <f t="shared" si="1"/>
-        <v>-51.488112746033423</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="3"/>
-        <v>0.62446290461185905</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8">
-        <v>701.2</v>
-      </c>
-      <c r="C9" s="8">
-        <v>215.1</v>
-      </c>
-      <c r="D9" s="7">
-        <v>38.17</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="10">
-        <f t="shared" si="4"/>
-        <v>-10.264029940685894</v>
-      </c>
-      <c r="I9" s="8">
-        <f t="shared" si="0"/>
-        <v>-10.362137382398966</v>
-      </c>
-      <c r="J9" s="8">
-        <f t="shared" si="2"/>
-        <v>-68.706000000000003</v>
-      </c>
-      <c r="K9" s="8">
-        <f t="shared" si="1"/>
-        <v>-72.343212848587157</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="3"/>
-        <v>0.30675984027381631</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8">
-        <v>700.9</v>
-      </c>
-      <c r="C10" s="8">
-        <v>112.6</v>
-      </c>
-      <c r="D10" s="7">
-        <v>21.63</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="10">
-        <f t="shared" si="4"/>
-        <v>-15.882353389364338</v>
-      </c>
-      <c r="I10" s="8">
-        <f t="shared" si="0"/>
-        <v>-16.072235265805517</v>
-      </c>
-      <c r="J10" s="8">
-        <f t="shared" si="2"/>
-        <v>-77.867999999999995</v>
-      </c>
-      <c r="K10" s="8">
-        <f t="shared" si="1"/>
-        <v>-80.956938920962315</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>0.16065059209587673</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>20</v>
-      </c>
-      <c r="B11" s="8">
-        <v>701.2</v>
-      </c>
-      <c r="C11" s="8">
-        <v>57.09</v>
-      </c>
-      <c r="D11" s="7">
-        <v>11.67</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="10">
-        <f t="shared" si="4"/>
-        <v>-21.785637288301487</v>
-      </c>
-      <c r="I11" s="8">
-        <f t="shared" si="0"/>
-        <v>-22.011612586390065</v>
-      </c>
-      <c r="J11" s="8">
-        <f t="shared" si="2"/>
-        <v>-84.024000000000001</v>
-      </c>
-      <c r="K11" s="8">
-        <f t="shared" si="1"/>
-        <v>-85.450134690878912</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="3"/>
-        <v>8.1417569880205362E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>50</v>
-      </c>
-      <c r="B12" s="8">
-        <v>701.4</v>
-      </c>
-      <c r="C12" s="8">
-        <v>23.5</v>
-      </c>
-      <c r="D12" s="7">
-        <v>4.782</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" si="4"/>
-        <v>-29.497957985474947</v>
-      </c>
-      <c r="I12" s="8">
-        <f t="shared" si="0"/>
-        <v>-29.947395549253176</v>
-      </c>
-      <c r="J12" s="8">
-        <f t="shared" si="2"/>
-        <v>-86.076000000000022</v>
-      </c>
-      <c r="K12" s="8">
-        <f t="shared" si="1"/>
-        <v>-88.176834279185869</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
-        <v>3.3504419731964642E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>100</v>
-      </c>
-      <c r="B13" s="8">
-        <v>700.9</v>
-      </c>
-      <c r="C13" s="8">
-        <v>11.97</v>
-      </c>
-      <c r="D13" s="7">
-        <v>2.8260000000000001</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="10">
-        <f t="shared" si="4"/>
-        <v>-35.35123819154267</v>
-      </c>
-      <c r="I13" s="8">
-        <f t="shared" si="0"/>
-        <v>-35.964697308632864</v>
-      </c>
-      <c r="J13" s="8">
-        <f t="shared" si="2"/>
-        <v>-101.73599999999999</v>
-      </c>
-      <c r="K13" s="8">
-        <f t="shared" si="1"/>
-        <v>-89.088186330386165</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
-        <v>1.7078042516764161E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="22">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="22">
+        <v>0.115</v>
+      </c>
     </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <f>0.1-0.015</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D25" s="1"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D27" s="1"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
     </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D28" s="1"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D29" s="1"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D30" s="1"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
     </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D31" s="1"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D32" s="1"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D33" s="1"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D34" s="1"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>